<commit_message>
Added tab for non-standard names
</commit_message>
<xml_diff>
--- a/BV paper data.xlsx
+++ b/BV paper data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrGJ/Documents/ShinyByGIT/BV-Shiny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2331281C-517E-5A45-A3F0-5B07D34E9C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D00CDED-72D0-3B4C-BF10-A71DEB4C5F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48460" yWindow="-4500" windowWidth="25600" windowHeight="20540" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48460" yWindow="-4500" windowWidth="25600" windowHeight="20540" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BVtable1.txt" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="BV flat.txt" sheetId="4" r:id="rId4"/>
     <sheet name="Small N BV" sheetId="13" r:id="rId5"/>
     <sheet name="Small N w zero BV" sheetId="14" r:id="rId6"/>
-    <sheet name="ECx  data.txt" sheetId="5" r:id="rId7"/>
-    <sheet name="ECx data + Bkgd.txt" sheetId="6" r:id="rId8"/>
-    <sheet name="ECx  data 4s.txt" sheetId="7" r:id="rId9"/>
-    <sheet name="ECx  data 3s.txt" sheetId="8" r:id="rId10"/>
-    <sheet name="ECx  data 2s.txt" sheetId="9" r:id="rId11"/>
-    <sheet name="ECx trouble" sheetId="10" r:id="rId12"/>
-    <sheet name="ECx error" sheetId="11" r:id="rId13"/>
-    <sheet name="ECx trouble + bkgd" sheetId="12" r:id="rId14"/>
+    <sheet name="Small N+zero+names" sheetId="15" r:id="rId7"/>
+    <sheet name="ECx  data.txt" sheetId="5" r:id="rId8"/>
+    <sheet name="ECx data + Bkgd.txt" sheetId="6" r:id="rId9"/>
+    <sheet name="ECx  data 4s.txt" sheetId="7" r:id="rId10"/>
+    <sheet name="ECx  data 3s.txt" sheetId="8" r:id="rId11"/>
+    <sheet name="ECx  data 2s.txt" sheetId="9" r:id="rId12"/>
+    <sheet name="ECx trouble" sheetId="10" r:id="rId13"/>
+    <sheet name="ECx error" sheetId="11" r:id="rId14"/>
+    <sheet name="ECx trouble + bkgd" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="7">
   <si>
     <t>y</t>
   </si>
@@ -53,6 +54,12 @@
   </si>
   <si>
     <t>sizes</t>
+  </si>
+  <si>
+    <t>yVar</t>
+  </si>
+  <si>
+    <t>doseVar</t>
   </si>
 </sst>
 </file>
@@ -649,6 +656,92 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -734,7 +827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -821,7 +914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -907,7 +1000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -993,7 +1086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1940,7 +2033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79146671-94AE-B84B-8F71-824C6B71BDE0}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2040,6 +2133,109 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03855E41-41A6-6A47-8819-C4F72702589B}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1.8</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1.3</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2110,101 +2306,6 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
         <v>20</v>
       </c>
     </row>
@@ -2219,12 +2320,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2241,57 +2340,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
       <c r="C5">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sheet with no data
</commit_message>
<xml_diff>
--- a/BV paper data.xlsx
+++ b/BV paper data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrGJ/Documents/ShinyByGIT/BV-Shiny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D00CDED-72D0-3B4C-BF10-A71DEB4C5F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E49AC5-D0EE-F248-B3A6-8118954680F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48460" yWindow="-4500" windowWidth="25600" windowHeight="20540" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48460" yWindow="-4500" windowWidth="25600" windowHeight="20540" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BVtable1.txt" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="BV flat.txt" sheetId="4" r:id="rId4"/>
     <sheet name="Small N BV" sheetId="13" r:id="rId5"/>
     <sheet name="Small N w zero BV" sheetId="14" r:id="rId6"/>
-    <sheet name="Small N+zero+names" sheetId="15" r:id="rId7"/>
-    <sheet name="ECx  data.txt" sheetId="5" r:id="rId8"/>
-    <sheet name="ECx data + Bkgd.txt" sheetId="6" r:id="rId9"/>
-    <sheet name="ECx  data 4s.txt" sheetId="7" r:id="rId10"/>
-    <sheet name="ECx  data 3s.txt" sheetId="8" r:id="rId11"/>
-    <sheet name="ECx  data 2s.txt" sheetId="9" r:id="rId12"/>
-    <sheet name="ECx trouble" sheetId="10" r:id="rId13"/>
-    <sheet name="ECx error" sheetId="11" r:id="rId14"/>
-    <sheet name="ECx trouble + bkgd" sheetId="12" r:id="rId15"/>
+    <sheet name="No data" sheetId="16" r:id="rId7"/>
+    <sheet name="Small N+zero+names" sheetId="15" r:id="rId8"/>
+    <sheet name="ECx  data.txt" sheetId="5" r:id="rId9"/>
+    <sheet name="ECx data + Bkgd.txt" sheetId="6" r:id="rId10"/>
+    <sheet name="ECx  data 4s.txt" sheetId="7" r:id="rId11"/>
+    <sheet name="ECx  data 3s.txt" sheetId="8" r:id="rId12"/>
+    <sheet name="ECx  data 2s.txt" sheetId="9" r:id="rId13"/>
+    <sheet name="ECx trouble" sheetId="10" r:id="rId14"/>
+    <sheet name="ECx error" sheetId="11" r:id="rId15"/>
+    <sheet name="ECx trouble + bkgd" sheetId="12" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>y</t>
   </si>
@@ -60,6 +61,27 @@
   </si>
   <si>
     <t>doseVar</t>
+  </si>
+  <si>
+    <t>There</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>hmm</t>
   </si>
 </sst>
 </file>
@@ -656,6 +678,101 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -741,7 +858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -827,7 +944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -914,7 +1031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1000,7 +1117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1086,7 +1203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2133,10 +2250,56 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01952393-81DB-A842-8DBD-E5D5FDD7D606}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03855E41-41A6-6A47-8819-C4F72702589B}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2235,7 +2398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2317,99 +2480,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>